<commit_message>
completed issues and factura
</commit_message>
<xml_diff>
--- a/Registers/Registro.xlsx
+++ b/Registers/Registro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tausand\TausandBill\Registers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A607D5FA-7E30-4B0A-A5A4-5A56314E29C5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA62CDC5-45FE-4E8D-864F-2CD144A332CF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -454,7 +454,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>